<commit_message>
arrow change, chart rename
</commit_message>
<xml_diff>
--- a/Excel_Data/Abbott_India.xlsx
+++ b/Excel_Data/Abbott_India.xlsx
@@ -60,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,9 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,8 +487,8 @@
       <c r="K2">
         <v>1632</v>
       </c>
-      <c r="L2">
-        <v>1600</v>
+      <c r="L2" s="2">
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>